<commit_message>
Modify DCF mapping spreadsheet
</commit_message>
<xml_diff>
--- a/Death Form Item to VRDR mappings.xlsx
+++ b/Death Form Item to VRDR mappings.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\AbdulMalikShakir\Documents\NCHS-20210126T065408Z-001\NCHS\VR_FHIR\VRDR_R4_Publication\vrdr\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CC14D179-1CC8-47D1-86A6-F3A5A1D1734D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{23D20F8B-91C8-4D8E-9A6F-89FEFE9A2B18}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-98" yWindow="-98" windowWidth="20715" windowHeight="13276" xr2:uid="{2B330604-515F-445F-862E-D97E7C4B29CB}"/>
   </bookViews>
@@ -1144,7 +1144,7 @@
   <sheetFormatPr defaultColWidth="14.3984375" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.45"/>
   <cols>
     <col min="1" max="1" width="23.265625" customWidth="1"/>
-    <col min="2" max="2" width="10.59765625" customWidth="1"/>
+    <col min="2" max="2" width="7.06640625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="57.265625" customWidth="1"/>
     <col min="4" max="4" width="49.59765625" customWidth="1"/>
     <col min="5" max="5" width="41.86328125" customWidth="1"/>

</xml_diff>

<commit_message>
Update to DCF mapping spreadsheet
</commit_message>
<xml_diff>
--- a/Death Form Item to VRDR mappings.xlsx
+++ b/Death Form Item to VRDR mappings.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\AbdulMalikShakir\Documents\NCHS-20210126T065408Z-001\NCHS\VR_FHIR\VRDR_R4_Publication\vrdr\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{23D20F8B-91C8-4D8E-9A6F-89FEFE9A2B18}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E8215D01-9F77-4B76-B636-9729AD403993}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-98" yWindow="-98" windowWidth="20715" windowHeight="13276" xr2:uid="{2B330604-515F-445F-862E-D97E7C4B29CB}"/>
   </bookViews>
@@ -1144,7 +1144,7 @@
   <sheetFormatPr defaultColWidth="14.3984375" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.45"/>
   <cols>
     <col min="1" max="1" width="23.265625" customWidth="1"/>
-    <col min="2" max="2" width="7.06640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="10.59765625" customWidth="1"/>
     <col min="3" max="3" width="57.265625" customWidth="1"/>
     <col min="4" max="4" width="49.59765625" customWidth="1"/>
     <col min="5" max="5" width="41.86328125" customWidth="1"/>

</xml_diff>

<commit_message>
minor change to vrdr mapping
</commit_message>
<xml_diff>
--- a/Death Form Item to VRDR mappings.xlsx
+++ b/Death Form Item to VRDR mappings.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\AbdulMalikShakir\Documents\NCHS-20210126T065408Z-001\NCHS\VR_FHIR\VRDR_R4_Publication\vrdr\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1438A149-A3AB-4FC1-B9BF-C92E9EA56780}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{625E0E40-90DC-4033-994A-B606916BE8DD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{2B330604-515F-445F-862E-D97E7C4B29CB}"/>
   </bookViews>
@@ -1138,7 +1138,7 @@
       <pane xSplit="2" ySplit="1" topLeftCell="C32" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="C35" sqref="C35"/>
+      <selection pane="bottomRight" activeCell="E1" sqref="E1:E1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -1147,7 +1147,7 @@
     <col min="2" max="2" width="10.5703125" customWidth="1"/>
     <col min="3" max="3" width="61.42578125" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="49.5703125" customWidth="1"/>
-    <col min="5" max="5" width="41.85546875" customWidth="1"/>
+    <col min="5" max="5" width="44.85546875" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="9.5703125" customWidth="1"/>
     <col min="7" max="25" width="9.140625" customWidth="1"/>
     <col min="26" max="26" width="13.42578125" customWidth="1"/>

</xml_diff>

<commit_message>
Update Death Form Item to VRDR mappings.xlsx
</commit_message>
<xml_diff>
--- a/Death Form Item to VRDR mappings.xlsx
+++ b/Death Form Item to VRDR mappings.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\AbdulMalikShakir\Documents\NCHS-20210126T065408Z-001\NCHS\VR_FHIR\VRDR_R4_Publication\vrdr\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{625E0E40-90DC-4033-994A-B606916BE8DD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BA5C76C9-0F52-4197-998C-B2DF30F5967F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{2B330604-515F-445F-862E-D97E7C4B29CB}"/>
   </bookViews>
@@ -1138,7 +1138,7 @@
       <pane xSplit="2" ySplit="1" topLeftCell="C32" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="E1" sqref="E1:E1048576"/>
+      <selection pane="bottomRight" activeCell="D1" sqref="D1:D1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -1146,7 +1146,7 @@
     <col min="1" max="1" width="23.28515625" customWidth="1"/>
     <col min="2" max="2" width="10.5703125" customWidth="1"/>
     <col min="3" max="3" width="61.42578125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="49.5703125" customWidth="1"/>
+    <col min="4" max="4" width="53.140625" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="44.85546875" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="9.5703125" customWidth="1"/>
     <col min="7" max="25" width="9.140625" customWidth="1"/>

</xml_diff>

<commit_message>
update dependencies in the PHINVADS branch
</commit_message>
<xml_diff>
--- a/Death Form Item to VRDR mappings.xlsx
+++ b/Death Form Item to VRDR mappings.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\AbdulMalikShakir\Documents\NCHS-20210126T065408Z-001\NCHS\VR_FHIR\VRDR_R4_Publication\vrdr\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BA5C76C9-0F52-4197-998C-B2DF30F5967F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{92608DFB-58E7-4DFB-B28E-6BFDFA791184}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{2B330604-515F-445F-862E-D97E7C4B29CB}"/>
   </bookViews>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="550" uniqueCount="154">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="550" uniqueCount="155">
   <si>
     <t>Subdomain</t>
   </si>
@@ -497,6 +497,9 @@
   </si>
   <si>
     <t>Organization.address</t>
+  </si>
+  <si>
+    <t>Item ID</t>
   </si>
 </sst>
 </file>
@@ -1138,13 +1141,13 @@
       <pane xSplit="2" ySplit="1" topLeftCell="C32" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="D1" sqref="D1:D1048576"/>
+      <selection pane="bottomRight" activeCell="C39" sqref="C39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="23.28515625" customWidth="1"/>
-    <col min="2" max="2" width="10.5703125" customWidth="1"/>
+    <col min="2" max="2" width="10.7109375" customWidth="1"/>
     <col min="3" max="3" width="61.42578125" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="53.140625" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="44.85546875" bestFit="1" customWidth="1"/>
@@ -1153,12 +1156,12 @@
     <col min="26" max="26" width="13.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:26" ht="17.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:26" ht="33" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>1</v>
+        <v>154</v>
       </c>
       <c r="C1" s="3" t="s">
         <v>2</v>

</xml_diff>